<commit_message>
Updated titles and font sizes on plots
</commit_message>
<xml_diff>
--- a/Analyzed data and scripts/exploData.xlsx
+++ b/Analyzed data and scripts/exploData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemfn\Documents\CWRU\R projects\StimTrailsAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documents\Unity Projects\CurrentProject\DR-SENS_Haptic_Feedback_JNE_Data\Analyzed data and scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330628C7-C016-4F40-9E75-C02B31164727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="10010" activeTab="7" xr2:uid="{86008A67-9B0A-490D-8D81-9755772E858C}"/>
+    <workbookView xWindow="2655" yWindow="2655" windowWidth="19200" windowHeight="10005" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -163,15 +162,6 @@
     <t>Perception Threshold</t>
   </si>
   <si>
-    <t>Sensation's envelope size</t>
-  </si>
-  <si>
-    <t>Most distal sensation</t>
-  </si>
-  <si>
-    <t>Sensation's vertical centroid</t>
-  </si>
-  <si>
     <t>sd</t>
   </si>
   <si>
@@ -186,11 +176,20 @@
   <si>
     <t>Maximum Comfortable</t>
   </si>
+  <si>
+    <t>Sensation's Vertical Centroid</t>
+  </si>
+  <si>
+    <t>Most Distal Sensation</t>
+  </si>
+  <si>
+    <t>Sensation's Envelope Size</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,22 +541,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EE897E-7F9F-42CF-B730-A630A7A2870F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -579,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -590,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -601,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -612,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -623,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -634,7 +633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -645,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -656,7 +655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -667,7 +666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -678,7 +677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -695,19 +694,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF617B90-C40A-487B-8BEC-EB67B2C8E4C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -721,7 +720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -736,7 +735,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -751,7 +750,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -766,7 +765,7 @@
         <v>73.076923076923066</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -781,7 +780,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -796,7 +795,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -811,7 +810,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -826,7 +825,7 @@
         <v>84.615384615384613</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -841,7 +840,7 @@
         <v>42.307692307692307</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -856,7 +855,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -871,7 +870,7 @@
         <v>53.846153846153847</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -886,7 +885,7 @@
         <v>53.846153846153847</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -901,7 +900,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -916,7 +915,7 @@
         <v>57.692307692307686</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -931,7 +930,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -946,7 +945,7 @@
         <v>73.076923076923066</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -961,7 +960,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -976,7 +975,7 @@
         <v>92.307692307692307</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -991,7 +990,7 @@
         <v>53.846153846153847</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1005,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>38.461538461538467</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>73.076923076923066</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>26.923076923076923</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>26.923076923076923</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>19.230769230769234</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>53.846153846153847</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1170,7 @@
         <v>57.692307692307686</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1186,7 +1185,7 @@
         <v>76.923076923076934</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1201,7 +1200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>42.307692307692307</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>46.153846153846153</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1261,7 +1260,7 @@
         <v>23.076923076923077</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1276,7 +1275,7 @@
         <v>69.230769230769226</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>42.307692307692307</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>23.076923076923077</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1320,7 @@
         <v>38.461538461538467</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1335,7 @@
         <v>19.230769230769234</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>15.384615384615385</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>80.769230769230774</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>76.923076923076934</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>84.615384615384613</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1411,7 +1410,7 @@
         <v>84.615384615384613</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -1426,7 +1425,7 @@
         <v>80.769230769230774</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>76.923076923076934</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -1456,7 +1455,7 @@
         <v>76.923076923076934</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>73.076923076923066</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1486,7 +1485,7 @@
         <v>92.307692307692307</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1516,7 +1515,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>76.923076923076934</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -1546,7 +1545,7 @@
         <v>69.230769230769226</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>73.076923076923066</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1576,7 +1575,7 @@
         <v>80.769230769230774</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>69.230769230769226</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -1606,7 +1605,7 @@
         <v>65.384615384615387</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -1621,7 +1620,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -1636,7 +1635,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>61.53846153846154</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1665,7 @@
         <v>65.384615384615387</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -1681,7 +1680,7 @@
         <v>69.230769230769226</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -1696,7 +1695,7 @@
         <v>92.307692307692307</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>65.384615384615387</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>38.461538461538467</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -1741,7 +1740,7 @@
         <v>69.230769230769226</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -1777,20 +1776,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024AF0C8-E0A6-4705-B483-D6EDA9804931}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>39.285714285714285</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>57.142857142857139</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1849,7 +1848,7 @@
         <v>55.357142857142861</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>67.857142857142861</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>57.142857142857139</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>91.666666666666657</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>60.416666666666664</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>92.708333333333343</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>78.125</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>26.666666666666668</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2035,23 +2034,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114721DF-AAF2-4A92-9D51-8C24DD2582D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -2074,7 +2073,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2100,7 +2099,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2126,7 +2125,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2152,7 +2151,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2179,7 +2178,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2205,7 +2204,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2231,7 +2230,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2257,7 +2256,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2284,7 +2283,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2310,7 +2309,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2336,7 +2335,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2362,7 +2361,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2389,7 +2388,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2415,7 +2414,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2441,7 +2440,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2467,7 +2466,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2494,7 +2493,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2520,7 +2519,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2546,7 +2545,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2572,7 +2571,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2599,7 +2598,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2625,7 +2624,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2651,7 +2650,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2677,7 +2676,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2704,7 +2703,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2730,7 +2729,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2756,7 +2755,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2782,7 +2781,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2809,7 +2808,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2835,7 +2834,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2861,7 +2860,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2887,7 +2886,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2914,7 +2913,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2940,7 +2939,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2966,7 +2965,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2992,7 +2991,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3019,7 +3018,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3045,7 +3044,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3071,7 +3070,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3097,7 +3096,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3124,7 +3123,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -3150,7 +3149,7 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -3176,7 +3175,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -3202,7 +3201,7 @@
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
@@ -3229,7 +3228,7 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
@@ -3255,7 +3254,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5</v>
       </c>
@@ -3281,7 +3280,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
@@ -3307,7 +3306,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5</v>
       </c>
@@ -3334,7 +3333,7 @@
       </c>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5</v>
       </c>
@@ -3360,7 +3359,7 @@
       </c>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5</v>
       </c>
@@ -3386,7 +3385,7 @@
       </c>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5</v>
       </c>
@@ -3412,7 +3411,7 @@
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5</v>
       </c>
@@ -3439,7 +3438,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5</v>
       </c>
@@ -3465,7 +3464,7 @@
       </c>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5</v>
       </c>
@@ -3491,7 +3490,7 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5</v>
       </c>
@@ -3517,7 +3516,7 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5</v>
       </c>
@@ -3550,25 +3549,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A537435-0846-4AB3-BB2C-2B9DB9B19BF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>18.181818181818183</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>27.27272727272727</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>5.6818181818181817</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>1.1363636363636365</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3715,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3739,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3764,7 +3763,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3789,7 +3788,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3814,7 +3813,7 @@
         <v>5.1724137931034484</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3839,7 +3838,7 @@
         <v>5.1724137931034484</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3864,7 +3863,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3889,7 +3888,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3914,7 +3913,7 @@
         <v>16.129032258064516</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -3939,7 +3938,7 @@
         <v>19.35483870967742</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3964,7 +3963,7 @@
         <v>7.1428571428571423</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3989,7 +3988,7 @@
         <v>40.476190476190474</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4014,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>5.2631578947368416</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>10.526315789473683</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -4114,7 +4113,7 @@
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -4139,7 +4138,7 @@
         <v>2.2471910112359552</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -4189,7 +4188,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>15.625</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -4239,7 +4238,7 @@
         <v>15.625</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
@@ -4264,7 +4263,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -4289,7 +4288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -4314,7 +4313,7 @@
         <v>11.111111111111111</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -4345,20 +4344,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D78990-B961-4767-9754-57DA3AE2EA7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4407,7 +4406,7 @@
         <v>40.909090909090914</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4433,7 +4432,7 @@
         <v>59.090909090909093</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4459,7 +4458,7 @@
         <v>6.8181818181818175</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4485,7 +4484,7 @@
         <v>93.181818181818173</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4511,7 +4510,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4537,7 +4536,7 @@
         <v>81.25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -4563,7 +4562,7 @@
         <v>10.344827586206897</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4589,7 +4588,7 @@
         <v>89.65517241379311</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -4615,7 +4614,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -4641,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -4667,7 +4666,7 @@
         <v>29.032258064516132</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>70.967741935483872</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -4719,7 +4718,7 @@
         <v>47.619047619047613</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4745,7 +4744,7 @@
         <v>52.380952380952387</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>83.333333333333343</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -4797,7 +4796,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4849,7 +4848,7 @@
         <v>84.210526315789465</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -4875,7 +4874,7 @@
         <v>3.3707865168539324</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -4901,7 +4900,7 @@
         <v>96.629213483146074</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -4927,7 +4926,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -4953,7 +4952,7 @@
         <v>83.333333333333343</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -4979,7 +4978,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>68.75</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>14.666666666666666</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -5057,7 +5056,7 @@
         <v>85.333333333333343</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -5115,16 +5114,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D92548-1ECF-4DDC-BE4B-12C6B9856F27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -5153,7 +5152,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5246,7 +5245,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5277,7 +5276,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -5308,7 +5307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5339,7 +5338,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5370,7 +5369,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5401,7 +5400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -5439,38 +5438,39 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA550D49-DD40-4E87-884C-D8874E8FA466}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
       </c>
       <c r="C2">
         <v>0.6</v>
@@ -5479,12 +5479,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>1.9090909089999999</v>
@@ -5493,12 +5493,12 @@
         <v>0.69090909099999998</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>2.7454545449999999</v>
@@ -5507,9 +5507,9 @@
         <v>0.83636363599999997</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -5521,9 +5521,9 @@
         <v>0.85636363599999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -5535,9 +5535,9 @@
         <v>0.70909090900000005</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>

</xml_diff>